<commit_message>
Added R style sheet for easier import
</commit_message>
<xml_diff>
--- a/ExampleData/dataForNormalizedIntensityCalc.xlsx
+++ b/ExampleData/dataForNormalizedIntensityCalc.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creuzige/Documents/NIST_Research/GitLab/austenitecalculator/ExampleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3173EE01-6D12-C04E-82E3-47AC37287F3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4AA977-3F35-6844-ABAB-806BCAB71FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40200" yWindow="4960" windowWidth="25880" windowHeight="13940" xr2:uid="{5546726D-3551-48BC-95FA-B28E8307A4AD}"/>
+    <workbookView xWindow="1260" yWindow="1200" windowWidth="33040" windowHeight="19160" activeTab="1" xr2:uid="{5546726D-3551-48BC-95FA-B28E8307A4AD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SpreadsheetFormat" sheetId="1" r:id="rId1"/>
+    <sheet name="RFormat" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="35">
   <si>
     <t>F</t>
   </si>
@@ -117,6 +118,27 @@
   </si>
   <si>
     <t>2theta</t>
+  </si>
+  <si>
+    <t>Param</t>
+  </si>
+  <si>
+    <t>Est Val</t>
+  </si>
+  <si>
+    <t>Uncer Val</t>
+  </si>
+  <si>
+    <t>Plane</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Austenite</t>
+  </si>
+  <si>
+    <t>Ferrite</t>
   </si>
 </sst>
 </file>
@@ -169,6 +191,1068 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Austenite</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SpreadsheetFormat!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SpreadsheetFormat!$B$14:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>295.204162999934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>261.3640272820976</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>294.81923412707147</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9446-8C41-8956-949878C43249}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ferrite</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SpreadsheetFormat!$H$2:$M$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>98.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SpreadsheetFormat!$H$14:$M$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>153.16907476796845</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>237.50577735218397</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>278.26176231269227</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9446-8C41-8956-949878C43249}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="174946960"/>
+        <c:axId val="174955968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="174946960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="40"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> Theta</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="174955968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="174955968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Normalized Intensity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="174946960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B781F9-0CB6-604F-9D7E-B2426AD988BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4EA8ED-0522-4E92-9B02-9317D9E49F40}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -977,5 +2061,1208 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1501EE83-3E4D-2B43-A6EA-5BF7FB9EEC5E}">
+  <dimension ref="A1:E73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>50.8</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>14.8</v>
+      </c>
+      <c r="C3">
+        <v>0.8</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>8.42</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.02</v>
+      </c>
+      <c r="C6">
+        <v>2E-3</v>
+      </c>
+      <c r="D6">
+        <v>200</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.05</v>
+      </c>
+      <c r="D7">
+        <v>200</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>200</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>45.26</v>
+      </c>
+      <c r="C10">
+        <v>2E-3</v>
+      </c>
+      <c r="D10">
+        <v>200</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>24514.799999999999</v>
+      </c>
+      <c r="C11">
+        <f>SQRT(B11)</f>
+        <v>156.57202815317939</v>
+      </c>
+      <c r="D11">
+        <v>200</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <f>((4*B3)^2)*B4*B5*EXP(-2*B6)*B7*B8*B9/(B10*B10)</f>
+        <v>83.043544341905104</v>
+      </c>
+      <c r="D12">
+        <v>200</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <f>B11/B12</f>
+        <v>295.204162999934</v>
+      </c>
+      <c r="D13">
+        <v>200</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="D14">
+        <v>220</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>0.8</v>
+      </c>
+      <c r="D15">
+        <v>220</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>220</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>3.66</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17">
+        <v>220</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>0.05</v>
+      </c>
+      <c r="C18">
+        <v>2E-3</v>
+      </c>
+      <c r="D18">
+        <v>220</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0.05</v>
+      </c>
+      <c r="D19">
+        <v>220</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0.05</v>
+      </c>
+      <c r="D20">
+        <v>220</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0.05</v>
+      </c>
+      <c r="D21">
+        <v>220</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>45.26</v>
+      </c>
+      <c r="C22">
+        <v>2E-3</v>
+      </c>
+      <c r="D22">
+        <v>220</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>11682.4</v>
+      </c>
+      <c r="C23">
+        <f>SQRT(B23)</f>
+        <v>108.08515161667674</v>
+      </c>
+      <c r="D23">
+        <v>220</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <f>((4*B15)^2)*B16*B17*EXP(-2*B18)*B19*B20*B21/(B22*B22)</f>
+        <v>44.697811406888277</v>
+      </c>
+      <c r="D24">
+        <v>220</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <f>B23/B24</f>
+        <v>261.3640272820976</v>
+      </c>
+      <c r="D25">
+        <v>220</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>90.6</v>
+      </c>
+      <c r="D26">
+        <v>311</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>10.7</v>
+      </c>
+      <c r="C27">
+        <v>0.8</v>
+      </c>
+      <c r="D27">
+        <v>311</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <v>311</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>2.8</v>
+      </c>
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>311</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>0.08</v>
+      </c>
+      <c r="C30">
+        <v>2E-3</v>
+      </c>
+      <c r="D30">
+        <v>311</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0.05</v>
+      </c>
+      <c r="D31">
+        <v>311</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0.05</v>
+      </c>
+      <c r="D32">
+        <v>311</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0.05</v>
+      </c>
+      <c r="D33">
+        <v>311</v>
+      </c>
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>45.26</v>
+      </c>
+      <c r="C34">
+        <v>2E-3</v>
+      </c>
+      <c r="D34">
+        <v>311</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>15097.2</v>
+      </c>
+      <c r="C35">
+        <f>SQRT(B35)</f>
+        <v>122.8706637078192</v>
+      </c>
+      <c r="D35">
+        <v>311</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36">
+        <f>((4*B27)^2)*B28*B29*EXP(-2*B30)*B31*B32*B33/(B34*B34)</f>
+        <v>51.208327857920168</v>
+      </c>
+      <c r="D36">
+        <v>311</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37">
+        <f>B35/B36</f>
+        <v>294.81923412707147</v>
+      </c>
+      <c r="D37">
+        <v>311</v>
+      </c>
+      <c r="E37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38">
+        <v>65</v>
+      </c>
+      <c r="D38">
+        <v>200</v>
+      </c>
+      <c r="E38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>14</v>
+      </c>
+      <c r="C39">
+        <v>0.8</v>
+      </c>
+      <c r="D39">
+        <v>200</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>200</v>
+      </c>
+      <c r="E40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>4.84</v>
+      </c>
+      <c r="C41">
+        <v>0.5</v>
+      </c>
+      <c r="D41">
+        <v>200</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C42">
+        <v>2E-3</v>
+      </c>
+      <c r="D42">
+        <v>200</v>
+      </c>
+      <c r="E42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>0.05</v>
+      </c>
+      <c r="D43">
+        <v>200</v>
+      </c>
+      <c r="E43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0.05</v>
+      </c>
+      <c r="D44">
+        <v>200</v>
+      </c>
+      <c r="E44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0.05</v>
+      </c>
+      <c r="D45">
+        <v>200</v>
+      </c>
+      <c r="E45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>24.192</v>
+      </c>
+      <c r="C46">
+        <v>2E-3</v>
+      </c>
+      <c r="D46">
+        <v>200</v>
+      </c>
+      <c r="E46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47">
+        <v>5445.7</v>
+      </c>
+      <c r="C47">
+        <f>SQRT(B47)</f>
+        <v>73.794986279556966</v>
+      </c>
+      <c r="D47">
+        <v>200</v>
+      </c>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48">
+        <f>((2*B39)^2)*B40*B41*EXP(-2*B42)*B43*B44*B45/(B46*B46)</f>
+        <v>35.553521546366575</v>
+      </c>
+      <c r="D48">
+        <v>200</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49">
+        <f>B47/B48</f>
+        <v>153.16907476796845</v>
+      </c>
+      <c r="D49">
+        <v>200</v>
+      </c>
+      <c r="E49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50">
+        <v>82.2</v>
+      </c>
+      <c r="D50">
+        <v>211</v>
+      </c>
+      <c r="E50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>11.8</v>
+      </c>
+      <c r="C51">
+        <v>0.8</v>
+      </c>
+      <c r="D51">
+        <v>211</v>
+      </c>
+      <c r="E51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>24</v>
+      </c>
+      <c r="D52">
+        <v>211</v>
+      </c>
+      <c r="E52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>3.13</v>
+      </c>
+      <c r="C53">
+        <v>0.5</v>
+      </c>
+      <c r="D53">
+        <v>211</v>
+      </c>
+      <c r="E53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C54">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D54">
+        <v>211</v>
+      </c>
+      <c r="E54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>0.05</v>
+      </c>
+      <c r="D55">
+        <v>211</v>
+      </c>
+      <c r="E55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0.05</v>
+      </c>
+      <c r="D56">
+        <v>211</v>
+      </c>
+      <c r="E56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>0.05</v>
+      </c>
+      <c r="D57">
+        <v>211</v>
+      </c>
+      <c r="E57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58">
+        <v>24.192</v>
+      </c>
+      <c r="C58">
+        <v>2E-3</v>
+      </c>
+      <c r="D58">
+        <v>211</v>
+      </c>
+      <c r="E58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59">
+        <v>14849.6</v>
+      </c>
+      <c r="C59">
+        <f>SQRT(B59)</f>
+        <v>121.85893483860755</v>
+      </c>
+      <c r="D59">
+        <v>211</v>
+      </c>
+      <c r="E59" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60">
+        <f>((2*B51)^2)*B52*B53*EXP(-2*B54)*B55*B56*B57/(B58*B58)</f>
+        <v>62.523110660926633</v>
+      </c>
+      <c r="D60">
+        <v>211</v>
+      </c>
+      <c r="E60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61">
+        <f>B59/B60</f>
+        <v>237.50577735218397</v>
+      </c>
+      <c r="D61">
+        <v>211</v>
+      </c>
+      <c r="E61" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62">
+        <v>98.9</v>
+      </c>
+      <c r="D62">
+        <v>220</v>
+      </c>
+      <c r="E62" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>10.3</v>
+      </c>
+      <c r="C63">
+        <v>0.8</v>
+      </c>
+      <c r="D63">
+        <v>220</v>
+      </c>
+      <c r="E63" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>12</v>
+      </c>
+      <c r="D64">
+        <v>220</v>
+      </c>
+      <c r="E64" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65">
+        <v>2.73</v>
+      </c>
+      <c r="C65">
+        <v>0.5</v>
+      </c>
+      <c r="D65">
+        <v>220</v>
+      </c>
+      <c r="E65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>0.08</v>
+      </c>
+      <c r="C66">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D66">
+        <v>220</v>
+      </c>
+      <c r="E66" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>0.05</v>
+      </c>
+      <c r="D67">
+        <v>220</v>
+      </c>
+      <c r="E67" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>0.05</v>
+      </c>
+      <c r="D68">
+        <v>220</v>
+      </c>
+      <c r="E68" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>0.05</v>
+      </c>
+      <c r="D69">
+        <v>220</v>
+      </c>
+      <c r="E69" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70">
+        <v>24.192</v>
+      </c>
+      <c r="C70">
+        <v>2E-3</v>
+      </c>
+      <c r="D70">
+        <v>220</v>
+      </c>
+      <c r="E70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71">
+        <v>5632.5</v>
+      </c>
+      <c r="C71">
+        <f>SQRT(B71)</f>
+        <v>75.049983344435191</v>
+      </c>
+      <c r="D71">
+        <v>220</v>
+      </c>
+      <c r="E71" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72">
+        <f>((2*B63)^2)*B64*B65*EXP(-2*B66)*B67*B68*B69/(B70*B70)</f>
+        <v>20.241731933223964</v>
+      </c>
+      <c r="D72">
+        <v>220</v>
+      </c>
+      <c r="E72" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73">
+        <f>B71/B72</f>
+        <v>278.26176231269227</v>
+      </c>
+      <c r="D73">
+        <v>220</v>
+      </c>
+      <c r="E73" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added script for Scattering Factor calculation
</commit_message>
<xml_diff>
--- a/ExampleData/dataForNormalizedIntensityCalc.xlsx
+++ b/ExampleData/dataForNormalizedIntensityCalc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creuzige/Documents/NIST_Research/GitLab/austenitecalculator/ExampleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4AA977-3F35-6844-ABAB-806BCAB71FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBC865D-853E-D14D-86AA-161545AC332A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1200" windowWidth="33040" windowHeight="19160" activeTab="1" xr2:uid="{5546726D-3551-48BC-95FA-B28E8307A4AD}"/>
+    <workbookView xWindow="1260" yWindow="1200" windowWidth="33040" windowHeight="19160" xr2:uid="{5546726D-3551-48BC-95FA-B28E8307A4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="SpreadsheetFormat" sheetId="1" r:id="rId1"/>
@@ -614,6 +614,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1554,7 +1585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4EA8ED-0522-4E92-9B02-9317D9E49F40}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -2069,7 +2100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1501EE83-3E4D-2B43-A6EA-5BF7FB9EEC5E}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>

</xml_diff>